<commit_message>
started userpage routes and fixed bugs
</commit_message>
<xml_diff>
--- a/sampledata.xlsx
+++ b/sampledata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesse Klein\Desktop\Uni Work\INFS3202\INFS3202\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesse\Desktop\Node Projects\INFS3202\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BF3035A-AD90-4CE8-885E-A9C4BF33610F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FCE6D05-0864-432D-BBC0-24A0C61CFFE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4114EBEE-0603-4BE1-BEED-6A94DCEA3C2B}"/>
+    <workbookView xWindow="-13740" yWindow="4590" windowWidth="21600" windowHeight="11385" xr2:uid="{4114EBEE-0603-4BE1-BEED-6A94DCEA3C2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,12 +30,309 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
+  <si>
+    <t>VIDEOS</t>
+  </si>
+  <si>
+    <t>CrashingSwine05</t>
+  </si>
+  <si>
+    <t>jd10999</t>
+  </si>
+  <si>
+    <t>Spacey Jane</t>
+  </si>
+  <si>
+    <t>Stella Donnelly</t>
+  </si>
+  <si>
+    <t>cartertheteacher.mp4</t>
+  </si>
+  <si>
+    <t>confidence.mp4</t>
+  </si>
+  <si>
+    <t>goonbois.mp4</t>
+  </si>
+  <si>
+    <t>jamescutting.mp4</t>
+  </si>
+  <si>
+    <t>mattpassedout.mp4</t>
+  </si>
+  <si>
+    <t>seasonsgreetings.mp4</t>
+  </si>
+  <si>
+    <t>headcold.mp4</t>
+  </si>
+  <si>
+    <t>goodgrief.mp4</t>
+  </si>
+  <si>
+    <t>goodforyou.mp4</t>
+  </si>
+  <si>
+    <t>Carter Does His Best</t>
+  </si>
+  <si>
+    <t>Confidence Man Live at Riverstage</t>
+  </si>
+  <si>
+    <t>On the way to the Valley!</t>
+  </si>
+  <si>
+    <t>James Cutting shapes to STIFI</t>
+  </si>
+  <si>
+    <t>Good For You - Live at Laneway</t>
+  </si>
+  <si>
+    <t>Good Grief - Live at Laneway</t>
+  </si>
+  <si>
+    <t>Head Cold - Official Video</t>
+  </si>
+  <si>
+    <t>Season's Greetings - Live Performance</t>
+  </si>
+  <si>
+    <t>Matt Has a Rough 21st</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Stella Donnelly - Season's Greetings. An exclusive live performance for Vevo. Watch Stella Donnelly's music videos: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://bit.ly/2UgiC0r</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF030303"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Follow Vevo Find us on Facebook: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>http://www.facebook.com/VEVOUK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF030303"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Follow us on Twitter: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>http://www.twitter.com/VEVO_UK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF030303"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Follow us on Instagram: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>http://instagram.com/Vevo_UK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF030303"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Follow Stella Donnelly: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.facebook.com/stellamusicb...</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF030303"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://twitter.com/stelladonnelly</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF030303"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.instagram.com/stelladonne...</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF030303"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.stelladonnelly.com</t>
+    </r>
+  </si>
+  <si>
+    <t>2020-15-03</t>
+  </si>
+  <si>
+    <t>USERINFOS</t>
+  </si>
+  <si>
+    <t>Ernas123</t>
+  </si>
+  <si>
+    <t>jesse10klein@gmail.com</t>
+  </si>
+  <si>
+    <t>jesse11klein@gmail.com</t>
+  </si>
+  <si>
+    <t>jesse12klein@gmail.com</t>
+  </si>
+  <si>
+    <t>jesse13klein@gmail.com</t>
+  </si>
+  <si>
+    <t>SUBSCRIPTIONS</t>
+  </si>
+  <si>
+    <t>Sounds awesome, wish I was there!</t>
+  </si>
+  <si>
+    <t>Rusted stovetop kettle boiling…</t>
+  </si>
+  <si>
+    <t>Poor bloke, hope he's alright</t>
+  </si>
+  <si>
+    <t>Let's go Matt!!!!</t>
+  </si>
+  <si>
+    <t>Such a beautiful voice</t>
+  </si>
+  <si>
+    <t>Up James and up the STIFI</t>
+  </si>
+  <si>
+    <t>Amazing voice, collab?</t>
+  </si>
+  <si>
+    <t>You guys need help</t>
+  </si>
+  <si>
+    <t>Great set guys</t>
+  </si>
+  <si>
+    <t>Carter could not get laid in a brothel mate</t>
+  </si>
+  <si>
+    <t>Ohhhh I remember this set!</t>
+  </si>
+  <si>
+    <t>COMMENTS</t>
+  </si>
+  <si>
+    <t>VIDEO VOTES</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF030303"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -58,13 +355,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -377,12 +679,809 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CFB892B-F3B9-43B8-B274-17D0C8F0DAFE}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D52" sqref="A41:D52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>9</v>
+      </c>
+      <c r="D31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>9</v>
+      </c>
+      <c r="D35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <v>8</v>
+      </c>
+      <c r="D36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>11</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>6</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="B44">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>6</v>
+      </c>
+      <c r="B46">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>7</v>
+      </c>
+      <c r="B47">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>8</v>
+      </c>
+      <c r="B48">
+        <v>8</v>
+      </c>
+      <c r="C48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>9</v>
+      </c>
+      <c r="B49">
+        <v>6</v>
+      </c>
+      <c r="C49" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>10</v>
+      </c>
+      <c r="B50">
+        <v>6</v>
+      </c>
+      <c r="C50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>11</v>
+      </c>
+      <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>12</v>
+      </c>
+      <c r="B52">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D13" r:id="rId1" xr:uid="{16FD5278-8C7F-449C-978D-ED54045A3B36}"/>
+    <hyperlink ref="D14" r:id="rId2" xr:uid="{3FF65564-9306-4D6C-A849-9D00246B3708}"/>
+    <hyperlink ref="D15" r:id="rId3" xr:uid="{FEEDA53B-6586-409A-BA9C-E9CDEABDBF27}"/>
+    <hyperlink ref="D16" r:id="rId4" xr:uid="{0CD3E049-FBE4-4EAE-A451-5965D57DA789}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>